<commit_message>
Create title and header rows
</commit_message>
<xml_diff>
--- a/CountriesList.xlsx
+++ b/CountriesList.xlsx
@@ -12,7 +12,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="660">
+  <si>
+    <t>Countries List</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Currencies</t>
+  </si>
   <si>
     <t>Afghanistan</t>
   </si>
@@ -2021,3513 +2036,3535 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:D251"/>
+  <dimension ref="A1:D252"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>652230.0</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>28748.0</v>
+        <v>652230.0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>2381741.0</v>
+        <v>28748.0</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>199.0</v>
+        <v>2381741.0</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>468.0</v>
+        <v>199.0</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>1246700.0</v>
+        <v>468.0</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>91.0</v>
+        <v>1246700.0</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" t="n">
-        <v>1.4E7</v>
+        <v>91.0</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>442.0</v>
+        <v>1.4E7</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="n">
+        <v>442.0</v>
+      </c>
+      <c r="D11" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2780400.0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" t="n">
-        <v>29743.0</v>
+        <v>2780400.0</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" t="n">
-        <v>180.0</v>
+        <v>29743.0</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" t="n">
-        <v>7692024.0</v>
+        <v>180.0</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="n">
-        <v>83871.0</v>
+        <v>7692024.0</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C16" t="n">
-        <v>86600.0</v>
+        <v>83871.0</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" t="n">
-        <v>13943.0</v>
+        <v>86600.0</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" t="n">
-        <v>765.0</v>
+        <v>13943.0</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" t="n">
-        <v>147570.0</v>
+        <v>765.0</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" t="n">
-        <v>430.0</v>
+        <v>147570.0</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C21" t="n">
-        <v>207600.0</v>
+        <v>430.0</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" t="n">
-        <v>30528.0</v>
+        <v>207600.0</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C23" t="n">
-        <v>22966.0</v>
+        <v>30528.0</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C24" t="n">
-        <v>112622.0</v>
+        <v>22966.0</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C25" t="n">
-        <v>54.0</v>
+        <v>112622.0</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C26" t="n">
-        <v>38394.0</v>
+        <v>54.0</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C27" t="n">
-        <v>1098581.0</v>
+        <v>38394.0</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C28" t="n">
-        <v>51209.0</v>
+        <v>1098581.0</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C29" t="n">
-        <v>582000.0</v>
+        <v>51209.0</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="C30" t="n">
-        <v>49.0</v>
+        <v>582000.0</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="C31" t="n">
-        <v>8515767.0</v>
+        <v>49.0</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C32" t="n">
-        <v>60.0</v>
+        <v>8515767.0</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C33" t="n">
-        <v>151.0</v>
+        <v>60.0</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C34" t="n">
-        <v>5765.0</v>
+        <v>151.0</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C35" t="n">
-        <v>110879.0</v>
+        <v>5765.0</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C36" t="n">
-        <v>272967.0</v>
+        <v>110879.0</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C37" t="n">
-        <v>27834.0</v>
+        <v>272967.0</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C38" t="n">
-        <v>181035.0</v>
+        <v>27834.0</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C39" t="n">
-        <v>475442.0</v>
+        <v>181035.0</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C40" t="n">
-        <v>9984670.0</v>
+        <v>475442.0</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C41" t="n">
-        <v>4033.0</v>
+        <v>9984670.0</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C42" t="n">
-        <v>328.0</v>
+        <v>4033.0</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C43" t="n">
-        <v>264.0</v>
+        <v>328.0</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C44" t="n">
-        <v>622984.0</v>
+        <v>264.0</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C45" t="n">
-        <v>1284000.0</v>
+        <v>622984.0</v>
       </c>
       <c r="D45" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C46" t="n">
-        <v>756102.0</v>
+        <v>1284000.0</v>
       </c>
       <c r="D46" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C47" t="n">
-        <v>9706961.0</v>
+        <v>756102.0</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C48" t="n">
-        <v>135.0</v>
+        <v>9706961.0</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C49" t="n">
-        <v>14.0</v>
+        <v>135.0</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C50" t="n">
-        <v>1141748.0</v>
+        <v>14.0</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C51" t="n">
-        <v>1862.0</v>
+        <v>1141748.0</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C52" t="n">
-        <v>236.0</v>
+        <v>1862.0</v>
       </c>
       <c r="D52" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C53" t="n">
-        <v>51100.0</v>
+        <v>236.0</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C54" t="n">
-        <v>56594.0</v>
+        <v>51100.0</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C55" t="n">
-        <v>109884.0</v>
+        <v>56594.0</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C56" t="n">
-        <v>444.0</v>
+        <v>109884.0</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C57" t="n">
-        <v>9251.0</v>
+        <v>444.0</v>
       </c>
       <c r="D57" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C58" t="n">
-        <v>78865.0</v>
+        <v>9251.0</v>
       </c>
       <c r="D58" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C59" t="n">
-        <v>2344858.0</v>
+        <v>78865.0</v>
       </c>
       <c r="D59" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C60" t="n">
-        <v>43094.0</v>
+        <v>2344858.0</v>
       </c>
       <c r="D60" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C61" t="n">
-        <v>23200.0</v>
+        <v>43094.0</v>
       </c>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C62" t="n">
-        <v>751.0</v>
+        <v>23200.0</v>
       </c>
       <c r="D62" t="s">
-        <v>20</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C63" t="n">
-        <v>48671.0</v>
+        <v>751.0</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C64" t="n">
-        <v>276841.0</v>
+        <v>48671.0</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C65" t="n">
-        <v>1002450.0</v>
+        <v>276841.0</v>
       </c>
       <c r="D65" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C66" t="n">
-        <v>21041.0</v>
+        <v>1002450.0</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C67" t="n">
-        <v>28051.0</v>
+        <v>21041.0</v>
       </c>
       <c r="D67" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C68" t="n">
-        <v>117600.0</v>
+        <v>28051.0</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C69" t="n">
-        <v>45227.0</v>
+        <v>117600.0</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C70" t="n">
-        <v>17364.0</v>
+        <v>45227.0</v>
       </c>
       <c r="D70" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C71" t="n">
-        <v>1104300.0</v>
+        <v>17364.0</v>
       </c>
       <c r="D71" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B72" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C72" t="n">
-        <v>12173.0</v>
+        <v>1104300.0</v>
       </c>
       <c r="D72" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C73" t="n">
-        <v>1393.0</v>
+        <v>12173.0</v>
       </c>
       <c r="D73" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B74" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C74" t="n">
-        <v>18272.0</v>
+        <v>1393.0</v>
       </c>
       <c r="D74" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C75" t="n">
-        <v>338424.0</v>
+        <v>18272.0</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B76" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C76" t="n">
-        <v>551695.0</v>
+        <v>338424.0</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B77" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C77" t="n">
-        <v>83534.0</v>
+        <v>551695.0</v>
       </c>
       <c r="D77" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B78" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C78" t="n">
-        <v>4167.0</v>
+        <v>83534.0</v>
       </c>
       <c r="D78" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B79" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C79" t="n">
-        <v>7747.0</v>
+        <v>4167.0</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B80" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C80" t="n">
-        <v>267668.0</v>
+        <v>7747.0</v>
       </c>
       <c r="D80" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B81" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C81" t="n">
-        <v>10689.0</v>
+        <v>267668.0</v>
       </c>
       <c r="D81" t="s">
-        <v>213</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B82" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C82" t="n">
-        <v>69700.0</v>
+        <v>10689.0</v>
       </c>
       <c r="D82" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C83" t="n">
-        <v>357114.0</v>
+        <v>69700.0</v>
       </c>
       <c r="D83" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B84" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C84" t="n">
-        <v>238533.0</v>
+        <v>357114.0</v>
       </c>
       <c r="D84" t="s">
-        <v>221</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B85" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C85" t="n">
-        <v>6.0</v>
+        <v>238533.0</v>
       </c>
       <c r="D85" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B86" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C86" t="n">
-        <v>131990.0</v>
+        <v>6.0</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C87" t="n">
-        <v>2166086.0</v>
+        <v>131990.0</v>
       </c>
       <c r="D87" t="s">
-        <v>161</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B88" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C88" t="n">
-        <v>344.0</v>
+        <v>2166086.0</v>
       </c>
       <c r="D88" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C89" t="n">
-        <v>1628.0</v>
+        <v>344.0</v>
       </c>
       <c r="D89" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B90" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C90" t="n">
-        <v>549.0</v>
+        <v>1628.0</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B91" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C91" t="n">
-        <v>108889.0</v>
+        <v>549.0</v>
       </c>
       <c r="D91" t="s">
-        <v>236</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B92" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C92" t="n">
-        <v>78.0</v>
+        <v>108889.0</v>
       </c>
       <c r="D92" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C93" t="n">
-        <v>245857.0</v>
+        <v>78.0</v>
       </c>
       <c r="D93" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B94" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C94" t="n">
-        <v>36125.0</v>
+        <v>245857.0</v>
       </c>
       <c r="D94" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B95" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C95" t="n">
-        <v>214969.0</v>
+        <v>36125.0</v>
       </c>
       <c r="D95" t="s">
-        <v>247</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C96" t="n">
-        <v>27750.0</v>
+        <v>214969.0</v>
       </c>
       <c r="D96" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
       <c r="C97" t="n">
-        <v>412.0</v>
+        <v>27750.0</v>
       </c>
       <c r="D97" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B98" t="s">
-        <v>253</v>
+        <v>27</v>
       </c>
       <c r="C98" t="n">
-        <v>112492.0</v>
+        <v>412.0</v>
       </c>
       <c r="D98" t="s">
-        <v>254</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B99" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C99" t="n">
-        <v>1104.0</v>
+        <v>112492.0</v>
       </c>
       <c r="D99" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B100" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C100" t="n">
-        <v>93028.0</v>
+        <v>1104.0</v>
       </c>
       <c r="D100" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B101" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C101" t="n">
-        <v>103000.0</v>
+        <v>93028.0</v>
       </c>
       <c r="D101" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B102" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C102" t="n">
-        <v>3287590.0</v>
+        <v>103000.0</v>
       </c>
       <c r="D102" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B103" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C103" t="n">
-        <v>1904569.0</v>
+        <v>3287590.0</v>
       </c>
       <c r="D103" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B104" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C104" t="n">
-        <v>1648195.0</v>
+        <v>1904569.0</v>
       </c>
       <c r="D104" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B105" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C105" t="n">
-        <v>438317.0</v>
+        <v>1648195.0</v>
       </c>
       <c r="D105" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B106" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C106" t="n">
-        <v>70273.0</v>
+        <v>438317.0</v>
       </c>
       <c r="D106" t="s">
-        <v>14</v>
+        <v>280</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B107" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C107" t="n">
-        <v>572.0</v>
+        <v>70273.0</v>
       </c>
       <c r="D107" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B108" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C108" t="n">
-        <v>20770.0</v>
+        <v>572.0</v>
       </c>
       <c r="D108" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B109" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C109" t="n">
-        <v>301336.0</v>
+        <v>20770.0</v>
       </c>
       <c r="D109" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B110" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C110" t="n">
-        <v>322463.0</v>
+        <v>301336.0</v>
       </c>
       <c r="D110" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B111" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C111" t="n">
-        <v>10991.0</v>
+        <v>322463.0</v>
       </c>
       <c r="D111" t="s">
-        <v>290</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B112" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C112" t="n">
-        <v>377930.0</v>
+        <v>10991.0</v>
       </c>
       <c r="D112" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B113" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C113" t="n">
-        <v>116.0</v>
+        <v>377930.0</v>
       </c>
       <c r="D113" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B114" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C114" t="n">
-        <v>89342.0</v>
+        <v>116.0</v>
       </c>
       <c r="D114" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B115" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C115" t="n">
-        <v>2724900.0</v>
+        <v>89342.0</v>
       </c>
       <c r="D115" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B116" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C116" t="n">
-        <v>580367.0</v>
+        <v>2724900.0</v>
       </c>
       <c r="D116" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B117" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C117" t="n">
-        <v>811.0</v>
+        <v>580367.0</v>
       </c>
       <c r="D117" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B118" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C118" t="n">
-        <v>10908.0</v>
+        <v>811.0</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>313</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B119" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C119" t="n">
-        <v>17818.0</v>
+        <v>10908.0</v>
       </c>
       <c r="D119" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B120" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C120" t="n">
-        <v>199951.0</v>
+        <v>17818.0</v>
       </c>
       <c r="D120" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B121" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C121" t="n">
-        <v>236800.0</v>
+        <v>199951.0</v>
       </c>
       <c r="D121" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B122" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C122" t="n">
-        <v>64559.0</v>
+        <v>236800.0</v>
       </c>
       <c r="D122" t="s">
-        <v>14</v>
+        <v>324</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B123" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C123" t="n">
-        <v>10452.0</v>
+        <v>64559.0</v>
       </c>
       <c r="D123" t="s">
-        <v>324</v>
+        <v>19</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B124" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C124" t="n">
-        <v>30355.0</v>
+        <v>10452.0</v>
       </c>
       <c r="D124" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B125" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C125" t="n">
-        <v>111369.0</v>
+        <v>30355.0</v>
       </c>
       <c r="D125" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B126" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C126" t="n">
-        <v>1759540.0</v>
+        <v>111369.0</v>
       </c>
       <c r="D126" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B127" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C127" t="n">
-        <v>160.0</v>
+        <v>1759540.0</v>
       </c>
       <c r="D127" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B128" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C128" t="n">
-        <v>65300.0</v>
+        <v>160.0</v>
       </c>
       <c r="D128" t="s">
-        <v>14</v>
+        <v>341</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B129" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C129" t="n">
-        <v>2586.0</v>
+        <v>65300.0</v>
       </c>
       <c r="D129" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B130" t="s">
-        <v>22</v>
+        <v>344</v>
       </c>
       <c r="C130" t="n">
-        <v>30.0</v>
+        <v>2586.0</v>
       </c>
       <c r="D130" t="s">
-        <v>341</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B131" t="s">
-        <v>343</v>
+        <v>27</v>
       </c>
       <c r="C131" t="n">
-        <v>587041.0</v>
+        <v>30.0</v>
       </c>
       <c r="D131" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B132" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C132" t="n">
-        <v>118484.0</v>
+        <v>587041.0</v>
       </c>
       <c r="D132" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B133" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C133" t="n">
-        <v>330803.0</v>
+        <v>118484.0</v>
       </c>
       <c r="D133" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B134" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C134" t="n">
-        <v>300.0</v>
+        <v>330803.0</v>
       </c>
       <c r="D134" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B135" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C135" t="n">
-        <v>1240192.0</v>
+        <v>300.0</v>
       </c>
       <c r="D135" t="s">
-        <v>64</v>
+        <v>358</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B136" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C136" t="n">
-        <v>316.0</v>
+        <v>1240192.0</v>
       </c>
       <c r="D136" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B137" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C137" t="n">
-        <v>181.0</v>
+        <v>316.0</v>
       </c>
       <c r="D137" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B138" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C138" t="n">
-        <v>1128.0</v>
+        <v>181.0</v>
       </c>
       <c r="D138" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B139" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C139" t="n">
-        <v>1030700.0</v>
+        <v>1128.0</v>
       </c>
       <c r="D139" t="s">
-        <v>364</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B140" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C140" t="n">
-        <v>2040.0</v>
+        <v>1030700.0</v>
       </c>
       <c r="D140" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B141" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C141" t="n">
-        <v>374.0</v>
+        <v>2040.0</v>
       </c>
       <c r="D141" t="s">
-        <v>14</v>
+        <v>372</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B142" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C142" t="n">
-        <v>1964375.0</v>
+        <v>374.0</v>
       </c>
       <c r="D142" t="s">
-        <v>372</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B143" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C143" t="n">
-        <v>702.0</v>
+        <v>1964375.0</v>
       </c>
       <c r="D143" t="s">
-        <v>11</v>
+        <v>377</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B144" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C144" t="n">
-        <v>33846.0</v>
+        <v>702.0</v>
       </c>
       <c r="D144" t="s">
-        <v>377</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B145" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="C145" t="n">
-        <v>2.02</v>
+        <v>33846.0</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
+        <v>382</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B146" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C146" t="n">
-        <v>1564110.0</v>
+        <v>2.02</v>
       </c>
       <c r="D146" t="s">
-        <v>381</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B147" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C147" t="n">
-        <v>13812.0</v>
+        <v>1564110.0</v>
       </c>
       <c r="D147" t="s">
-        <v>14</v>
+        <v>386</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B148" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C148" t="n">
-        <v>102.0</v>
+        <v>13812.0</v>
       </c>
       <c r="D148" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B149" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C149" t="n">
-        <v>446550.0</v>
+        <v>102.0</v>
       </c>
       <c r="D149" t="s">
-        <v>388</v>
+        <v>25</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B150" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C150" t="n">
-        <v>801590.0</v>
+        <v>446550.0</v>
       </c>
       <c r="D150" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B151" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C151" t="n">
-        <v>676578.0</v>
+        <v>801590.0</v>
       </c>
       <c r="D151" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B152" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C152" t="n">
-        <v>825615.0</v>
+        <v>676578.0</v>
       </c>
       <c r="D152" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B153" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C153" t="n">
-        <v>21.0</v>
+        <v>825615.0</v>
       </c>
       <c r="D153" t="s">
-        <v>36</v>
+        <v>402</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B154" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C154" t="n">
-        <v>147181.0</v>
+        <v>21.0</v>
       </c>
       <c r="D154" t="s">
-        <v>402</v>
+        <v>41</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B155" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C155" t="n">
-        <v>41850.0</v>
+        <v>147181.0</v>
       </c>
       <c r="D155" t="s">
-        <v>14</v>
+        <v>407</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B156" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C156" t="n">
-        <v>18575.0</v>
+        <v>41850.0</v>
       </c>
       <c r="D156" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B157" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C157" t="n">
-        <v>270467.0</v>
+        <v>18575.0</v>
       </c>
       <c r="D157" t="s">
-        <v>409</v>
+        <v>211</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B158" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C158" t="n">
-        <v>130373.0</v>
+        <v>270467.0</v>
       </c>
       <c r="D158" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B159" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C159" t="n">
-        <v>1267000.0</v>
+        <v>130373.0</v>
       </c>
       <c r="D159" t="s">
-        <v>64</v>
+        <v>417</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B160" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C160" t="n">
-        <v>923768.0</v>
+        <v>1267000.0</v>
       </c>
       <c r="D160" t="s">
-        <v>417</v>
+        <v>69</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B161" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C161" t="n">
-        <v>260.0</v>
+        <v>923768.0</v>
       </c>
       <c r="D161" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B162" t="s">
-        <v>289</v>
+        <v>424</v>
       </c>
       <c r="C162" t="n">
-        <v>36.0</v>
+        <v>260.0</v>
       </c>
       <c r="D162" t="s">
-        <v>36</v>
+        <v>414</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B163" t="s">
-        <v>422</v>
+        <v>294</v>
       </c>
       <c r="C163" t="n">
-        <v>120538.0</v>
+        <v>36.0</v>
       </c>
       <c r="D163" t="s">
-        <v>423</v>
+        <v>41</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B164" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C164" t="n">
-        <v>25713.0</v>
+        <v>120538.0</v>
       </c>
       <c r="D164" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B165" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C165" t="n">
-        <v>464.0</v>
+        <v>25713.0</v>
       </c>
       <c r="D165" t="s">
-        <v>11</v>
+        <v>431</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B166" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C166" t="n">
-        <v>323802.0</v>
+        <v>464.0</v>
       </c>
       <c r="D166" t="s">
-        <v>431</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B167" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C167" t="n">
-        <v>309500.0</v>
+        <v>323802.0</v>
       </c>
       <c r="D167" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B168" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C168" t="n">
-        <v>881912.0</v>
+        <v>309500.0</v>
       </c>
       <c r="D168" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B169" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C169" t="n">
-        <v>459.0</v>
+        <v>881912.0</v>
       </c>
       <c r="D169" t="s">
-        <v>11</v>
+        <v>442</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B170" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C170" t="n">
-        <v>6220.0</v>
+        <v>459.0</v>
       </c>
       <c r="D170" t="s">
-        <v>442</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B171" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C171" t="n">
-        <v>75417.0</v>
+        <v>6220.0</v>
       </c>
       <c r="D171" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B172" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C172" t="n">
-        <v>462840.0</v>
+        <v>75417.0</v>
       </c>
       <c r="D172" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B173" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C173" t="n">
-        <v>406752.0</v>
+        <v>462840.0</v>
       </c>
       <c r="D173" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B174" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C174" t="n">
-        <v>1285216.0</v>
+        <v>406752.0</v>
       </c>
       <c r="D174" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B175" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C175" t="n">
-        <v>342353.0</v>
+        <v>1285216.0</v>
       </c>
       <c r="D175" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B176" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C176" t="n">
-        <v>47.0</v>
+        <v>342353.0</v>
       </c>
       <c r="D176" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B177" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C177" t="n">
-        <v>312679.0</v>
+        <v>47.0</v>
       </c>
       <c r="D177" t="s">
-        <v>462</v>
+        <v>414</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B178" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C178" t="n">
-        <v>92090.0</v>
+        <v>312679.0</v>
       </c>
       <c r="D178" t="s">
-        <v>14</v>
+        <v>467</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B179" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C179" t="n">
-        <v>8870.0</v>
+        <v>92090.0</v>
       </c>
       <c r="D179" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B180" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C180" t="n">
-        <v>11586.0</v>
+        <v>8870.0</v>
       </c>
       <c r="D180" t="s">
-        <v>469</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B181" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C181" t="n">
-        <v>342000.0</v>
+        <v>11586.0</v>
       </c>
       <c r="D181" t="s">
-        <v>104</v>
+        <v>474</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B182" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C182" t="n">
-        <v>238391.0</v>
+        <v>342000.0</v>
       </c>
       <c r="D182" t="s">
-        <v>474</v>
+        <v>109</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B183" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C183" t="n">
-        <v>1.7098242E7</v>
+        <v>238391.0</v>
       </c>
       <c r="D183" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B184" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C184" t="n">
-        <v>26338.0</v>
+        <v>1.7098242E7</v>
       </c>
       <c r="D184" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B185" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C185" t="n">
-        <v>2511.0</v>
+        <v>26338.0</v>
       </c>
       <c r="D185" t="s">
-        <v>14</v>
+        <v>485</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B186" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C186" t="n">
-        <v>21.0</v>
+        <v>2511.0</v>
       </c>
       <c r="D186" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B187" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C187" t="n">
-        <v>394.0</v>
+        <v>21.0</v>
       </c>
       <c r="D187" t="s">
-        <v>487</v>
+        <v>19</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B188" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C188" t="n">
-        <v>261.0</v>
+        <v>394.0</v>
       </c>
       <c r="D188" t="s">
-        <v>20</v>
+        <v>492</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B189" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="C189" t="n">
-        <v>616.0</v>
+        <v>261.0</v>
       </c>
       <c r="D189" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B190" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="C190" t="n">
-        <v>53.0</v>
+        <v>616.0</v>
       </c>
       <c r="D190" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B191" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C191" t="n">
-        <v>242.0</v>
+        <v>53.0</v>
       </c>
       <c r="D191" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B192" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="C192" t="n">
-        <v>389.0</v>
+        <v>242.0</v>
       </c>
       <c r="D192" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B193" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C193" t="n">
-        <v>2842.0</v>
+        <v>389.0</v>
       </c>
       <c r="D193" t="s">
-        <v>500</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B194" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C194" t="n">
-        <v>61.0</v>
+        <v>2842.0</v>
       </c>
       <c r="D194" t="s">
-        <v>14</v>
+        <v>505</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B195" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C195" t="n">
-        <v>2149690.0</v>
+        <v>61.0</v>
       </c>
       <c r="D195" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B196" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C196" t="n">
-        <v>196722.0</v>
+        <v>2149690.0</v>
       </c>
       <c r="D196" t="s">
-        <v>64</v>
+        <v>510</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B197" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C197" t="n">
-        <v>88361.0</v>
+        <v>196722.0</v>
       </c>
       <c r="D197" t="s">
-        <v>510</v>
+        <v>69</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B198" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C198" t="n">
-        <v>452.0</v>
+        <v>88361.0</v>
       </c>
       <c r="D198" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B199" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C199" t="n">
-        <v>71740.0</v>
+        <v>452.0</v>
       </c>
       <c r="D199" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B200" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C200" t="n">
-        <v>710.0</v>
+        <v>71740.0</v>
       </c>
       <c r="D200" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="B201" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C201" t="n">
-        <v>34.0</v>
+        <v>710.0</v>
       </c>
       <c r="D201" t="s">
-        <v>150</v>
+        <v>523</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B202" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C202" t="n">
-        <v>49037.0</v>
+        <v>34.0</v>
       </c>
       <c r="D202" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B203" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C203" t="n">
-        <v>20273.0</v>
+        <v>49037.0</v>
       </c>
       <c r="D203" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="B204" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C204" t="n">
-        <v>28896.0</v>
+        <v>20273.0</v>
       </c>
       <c r="D204" t="s">
-        <v>527</v>
+        <v>19</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B205" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C205" t="n">
-        <v>637657.0</v>
+        <v>28896.0</v>
       </c>
       <c r="D205" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B206" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C206" t="n">
-        <v>1221037.0</v>
+        <v>637657.0</v>
       </c>
       <c r="D206" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B207" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C207" t="n">
-        <v>3903.0</v>
+        <v>1221037.0</v>
       </c>
       <c r="D207" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B208" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C208" t="n">
-        <v>100210.0</v>
+        <v>3903.0</v>
       </c>
       <c r="D208" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B209" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C209" t="n">
-        <v>619745.0</v>
+        <v>100210.0</v>
       </c>
       <c r="D209" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B210" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C210" t="n">
-        <v>505992.0</v>
+        <v>619745.0</v>
       </c>
       <c r="D210" t="s">
-        <v>14</v>
+        <v>547</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B211" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C211" t="n">
-        <v>65610.0</v>
+        <v>505992.0</v>
       </c>
       <c r="D211" t="s">
-        <v>547</v>
+        <v>19</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B212" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C212" t="n">
-        <v>1886068.0</v>
+        <v>65610.0</v>
       </c>
       <c r="D212" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B213" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C213" t="n">
-        <v>163820.0</v>
+        <v>1886068.0</v>
       </c>
       <c r="D213" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B214" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C214" t="n">
-        <v>-1.0</v>
+        <v>163820.0</v>
       </c>
       <c r="D214" t="s">
-        <v>431</v>
+        <v>558</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="B215" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="C215" t="n">
-        <v>450295.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D215" t="s">
-        <v>558</v>
+        <v>436</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B216" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C216" t="n">
-        <v>41284.0</v>
+        <v>450295.0</v>
       </c>
       <c r="D216" t="s">
-        <v>336</v>
+        <v>563</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B217" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C217" t="n">
-        <v>185180.0</v>
+        <v>41284.0</v>
       </c>
       <c r="D217" t="s">
-        <v>563</v>
+        <v>341</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B218" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C218" t="n">
-        <v>964.0</v>
+        <v>185180.0</v>
       </c>
       <c r="D218" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B219" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C219" t="n">
-        <v>36193.0</v>
+        <v>964.0</v>
       </c>
       <c r="D219" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B220" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C220" t="n">
-        <v>143100.0</v>
+        <v>36193.0</v>
       </c>
       <c r="D220" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B221" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C221" t="n">
-        <v>945087.0</v>
+        <v>143100.0</v>
       </c>
       <c r="D221" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B222" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C222" t="n">
-        <v>513120.0</v>
+        <v>945087.0</v>
       </c>
       <c r="D222" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B223" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C223" t="n">
-        <v>14874.0</v>
+        <v>513120.0</v>
       </c>
       <c r="D223" t="s">
-        <v>11</v>
+        <v>583</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B224" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C224" t="n">
-        <v>56785.0</v>
+        <v>14874.0</v>
       </c>
       <c r="D224" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B225" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="C225" t="n">
-        <v>12.0</v>
+        <v>56785.0</v>
       </c>
       <c r="D225" t="s">
-        <v>409</v>
+        <v>69</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B226" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="C226" t="n">
-        <v>747.0</v>
+        <v>12.0</v>
       </c>
       <c r="D226" t="s">
-        <v>587</v>
+        <v>414</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B227" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C227" t="n">
-        <v>5130.0</v>
+        <v>747.0</v>
       </c>
       <c r="D227" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B228" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C228" t="n">
-        <v>163610.0</v>
+        <v>5130.0</v>
       </c>
       <c r="D228" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B229" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C229" t="n">
-        <v>783562.0</v>
+        <v>163610.0</v>
       </c>
       <c r="D229" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B230" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C230" t="n">
-        <v>488100.0</v>
+        <v>783562.0</v>
       </c>
       <c r="D230" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B231" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C231" t="n">
-        <v>948.0</v>
+        <v>488100.0</v>
       </c>
       <c r="D231" t="s">
-        <v>11</v>
+        <v>604</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="B232" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="C232" t="n">
-        <v>26.0</v>
+        <v>948.0</v>
       </c>
       <c r="D232" t="s">
-        <v>604</v>
+        <v>16</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B233" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C233" t="n">
-        <v>241550.0</v>
+        <v>26.0</v>
       </c>
       <c r="D233" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B234" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C234" t="n">
-        <v>603500.0</v>
+        <v>241550.0</v>
       </c>
       <c r="D234" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B235" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C235" t="n">
-        <v>83600.0</v>
+        <v>603500.0</v>
       </c>
       <c r="D235" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B236" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C236" t="n">
-        <v>242900.0</v>
+        <v>83600.0</v>
       </c>
       <c r="D236" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B237" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C237" t="n">
-        <v>9372610.0</v>
+        <v>242900.0</v>
       </c>
       <c r="D237" t="s">
-        <v>11</v>
+        <v>621</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="B238" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C238" t="n">
-        <v>34.2</v>
+        <v>9372610.0</v>
       </c>
       <c r="D238" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="B239" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="C239" t="n">
-        <v>347.0</v>
+        <v>34.2</v>
       </c>
       <c r="D239" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B240" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="C240" t="n">
-        <v>181034.0</v>
+        <v>347.0</v>
       </c>
       <c r="D240" t="s">
-        <v>625</v>
+        <v>16</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B241" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="C241" t="n">
-        <v>447400.0</v>
+        <v>181034.0</v>
       </c>
       <c r="D241" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B242" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C242" t="n">
-        <v>12189.0</v>
+        <v>447400.0</v>
       </c>
       <c r="D242" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B243" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C243" t="n">
-        <v>0.44</v>
+        <v>12189.0</v>
       </c>
       <c r="D243" t="s">
-        <v>14</v>
+        <v>636</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="B244" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C244" t="n">
-        <v>916445.0</v>
+        <v>0.44</v>
       </c>
       <c r="D244" t="s">
-        <v>635</v>
+        <v>19</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B245" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C245" t="n">
-        <v>331212.0</v>
+        <v>916445.0</v>
       </c>
       <c r="D245" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B246" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C246" t="n">
-        <v>142.0</v>
+        <v>331212.0</v>
       </c>
       <c r="D246" t="s">
-        <v>206</v>
+        <v>643</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B247" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C247" t="n">
-        <v>266000.0</v>
+        <v>142.0</v>
       </c>
       <c r="D247" t="s">
-        <v>643</v>
+        <v>211</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B248" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C248" t="n">
-        <v>527968.0</v>
+        <v>266000.0</v>
       </c>
       <c r="D248" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B249" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C249" t="n">
-        <v>752612.0</v>
+        <v>527968.0</v>
       </c>
       <c r="D249" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B250" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="C250" t="n">
-        <v>390757.0</v>
+        <v>752612.0</v>
       </c>
       <c r="D250" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B251" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C251" t="n">
+        <v>390757.0</v>
+      </c>
+      <c r="D251" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>658</v>
+      </c>
+      <c r="B252" t="s">
+        <v>659</v>
+      </c>
+      <c r="C252" t="n">
         <v>1580.0</v>
       </c>
-      <c r="D251" t="s">
-        <v>14</v>
+      <c r="D252" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>